<commit_message>
refactor: update demo data and csv file for testing
</commit_message>
<xml_diff>
--- a/src/test/resources/issue/common/simple.xlsx
+++ b/src/test/resources/issue/common/simple.xlsx
@@ -4,11 +4,10 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="25280" activeTab="1"/>
+    <workbookView windowHeight="27520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,75 +27,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t>字符串标题</t>
+    <t>StringTitle</t>
   </si>
   <si>
-    <t>日期标题</t>
+    <t>DateTitle</t>
   </si>
   <si>
-    <t>数字标题</t>
+    <t>DoubleTitle</t>
   </si>
   <si>
-    <t>String10</t>
+    <t xml:space="preserve">String10 </t>
   </si>
   <si>
-    <t>String11</t>
+    <t xml:space="preserve">String11 </t>
   </si>
   <si>
-    <t>String12</t>
+    <t xml:space="preserve">String12 </t>
   </si>
   <si>
-    <t>String13</t>
+    <t xml:space="preserve">String13 </t>
   </si>
   <si>
-    <t>String14</t>
+    <t xml:space="preserve">String14 </t>
   </si>
   <si>
-    <t>String15</t>
+    <t>String15　</t>
   </si>
   <si>
-    <t>String16</t>
+    <t>String16　</t>
   </si>
   <si>
-    <t>String17</t>
+    <t>String17　</t>
   </si>
   <si>
-    <t>String18</t>
+    <t xml:space="preserve">String18 </t>
   </si>
   <si>
-    <t>String19</t>
-  </si>
-  <si>
-    <t>String20</t>
-  </si>
-  <si>
-    <t>String21</t>
-  </si>
-  <si>
-    <t>String22</t>
-  </si>
-  <si>
-    <t>String23</t>
-  </si>
-  <si>
-    <t>String24</t>
-  </si>
-  <si>
-    <t>String25</t>
-  </si>
-  <si>
-    <t>String26</t>
-  </si>
-  <si>
-    <t>String27</t>
-  </si>
-  <si>
-    <t>String28</t>
-  </si>
-  <si>
-    <t>String29</t>
+    <t xml:space="preserve">String19 </t>
   </si>
 </sst>
 </file>
@@ -1254,8 +1223,8 @@
   <sheetPr/>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.3846153846154" defaultRowHeight="16.8" outlineLevelCol="2"/>
@@ -1389,146 +1358,4 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:C11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="2"/>
-  <cols>
-    <col min="1" max="1" width="12.7692307692308" customWidth="1"/>
-    <col min="2" max="2" width="15.3846153846154" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="1">
-        <v>43831.0423611111</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1">
-        <v>43832.0423611111</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="1">
-        <v>43833.0423611111</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1">
-        <v>43834.0423611111</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="1">
-        <v>43835.0423611111</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="1">
-        <v>43836.0423611111</v>
-      </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="1">
-        <v>43837.0423611111</v>
-      </c>
-      <c r="C8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="1">
-        <v>43838.0423611111</v>
-      </c>
-      <c r="C9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="1">
-        <v>43839.0423611111</v>
-      </c>
-      <c r="C10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="1">
-        <v>43840.0423611111</v>
-      </c>
-      <c r="C11">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
test(fastexcel): add unit test for issue 564
</commit_message>
<xml_diff>
--- a/src/test/resources/issue/common/simple.xlsx
+++ b/src/test/resources/issue/common/simple.xlsx
@@ -685,7 +685,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="31" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1224,7 +1224,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.3846153846154" defaultRowHeight="16.8" outlineLevelCol="2"/>

</xml_diff>